<commit_message>
Add Pregnancy Registration feature
</commit_message>
<xml_diff>
--- a/app/src/main/res/raw/pregnancy_registration_form.xlsx
+++ b/app/src/main/res/raw/pregnancy_registration_form.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowHeight="17670" tabRatio="500"/>
+    <workbookView windowHeight="17730" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="columns" sheetId="1" r:id="rId1"/>
@@ -50,7 +50,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="153" uniqueCount="117">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="156" uniqueCount="119">
   <si>
     <t>group</t>
   </si>
@@ -256,7 +256,7 @@
     <t>5. Data provável do parto pre-calculada</t>
   </si>
   <si>
-    <t>call:calculateEdd(${eddDate}, ${lmpDate},${pregMonths})</t>
+    <t>call:calculateEdd(${recordedDate}, ${eddDate}, ${lmpDate},${pregMonths})</t>
   </si>
   <si>
     <t>collected</t>
@@ -298,12 +298,18 @@
     <t>value</t>
   </si>
   <si>
+    <t>TRUE</t>
+  </si>
+  <si>
     <t>Yes</t>
   </si>
   <si>
     <t>Sim</t>
   </si>
   <si>
+    <t>FALSE</t>
+  </si>
+  <si>
     <t>No</t>
   </si>
   <si>
@@ -394,13 +400,13 @@
     <t>form_name::pt</t>
   </si>
   <si>
-    <t>rawChangeHead</t>
-  </si>
-  <si>
-    <t>Change of Head of Household</t>
-  </si>
-  <si>
-    <t>Mudança do chefe do agregado</t>
+    <t>rawPregnancyRegistration</t>
+  </si>
+  <si>
+    <t>Pregnancy Registration</t>
+  </si>
+  <si>
+    <t>Registo de Gravidez</t>
   </si>
 </sst>
 </file>
@@ -408,10 +414,10 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="4">
-    <numFmt numFmtId="176" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
     <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
+    <numFmt numFmtId="176" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
     <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
-    <numFmt numFmtId="177" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
+    <numFmt numFmtId="177" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
   </numFmts>
   <fonts count="28">
     <font>
@@ -447,6 +453,120 @@
       <sz val="10"/>
       <name val="Arial"/>
       <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="Arial"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFFFFFF"/>
+      <name val="Arial"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Arial"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Arial"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="15"/>
+      <color theme="3"/>
+      <name val="Arial"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="18"/>
+      <color theme="3"/>
+      <name val="Arial"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="3"/>
+      <name val="Arial"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Arial"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Arial"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF3F3F3F"/>
+      <name val="Arial"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="Arial"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF800080"/>
+      <name val="Arial"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
+      <name val="Arial"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color rgb="FF7F7F7F"/>
+      <name val="Arial"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Arial"/>
+      <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -459,9 +579,9 @@
     </font>
     <font>
       <sz val="11"/>
-      <color theme="1"/>
-      <name val="Arial"/>
-      <charset val="134"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Arial"/>
+      <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -473,129 +593,15 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <u/>
       <sz val="11"/>
-      <color rgb="FF800080"/>
+      <color rgb="FF9C6500"/>
       <name val="Arial"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
-      <sz val="18"/>
-      <color theme="3"/>
-      <name val="Arial"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="15"/>
-      <color theme="3"/>
-      <name val="Arial"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Arial"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF006100"/>
-      <name val="Arial"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Arial"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <sz val="11"/>
       <color rgb="FF3F3F76"/>
-      <name val="Arial"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="3"/>
-      <name val="Arial"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="0"/>
-      <name val="Arial"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
-      <name val="Arial"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C6500"/>
-      <name val="Arial"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
-      <name val="Arial"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <i/>
-      <sz val="11"/>
-      <color rgb="FF7F7F7F"/>
-      <name val="Arial"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Arial"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Arial"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFF0000"/>
-      <name val="Arial"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C0006"/>
       <name val="Arial"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -621,187 +627,187 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="9" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor rgb="FFC6EFCE"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="4" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -815,11 +821,35 @@
       <diagonal/>
     </border>
     <border>
+      <left style="double">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="double">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="double">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="double">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
       <left/>
       <right/>
       <top/>
       <bottom style="medium">
         <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4" tint="0.499984740745262"/>
       </bottom>
       <diagonal/>
     </border>
@@ -839,11 +869,17 @@
       <diagonal/>
     </border>
     <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4" tint="0.499984740745262"/>
+      <left style="thin">
+        <color rgb="FFB2B2B2"/>
+      </left>
+      <right style="thin">
+        <color rgb="FFB2B2B2"/>
+      </right>
+      <top style="thin">
+        <color rgb="FFB2B2B2"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FFB2B2B2"/>
       </bottom>
       <diagonal/>
     </border>
@@ -863,32 +899,13 @@
       <diagonal/>
     </border>
     <border>
-      <left style="double">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="double">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="double">
-        <color rgb="FF3F3F3F"/>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color theme="4"/>
       </top>
       <bottom style="double">
-        <color rgb="FF3F3F3F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FFB2B2B2"/>
-      </left>
-      <right style="thin">
-        <color rgb="FFB2B2B2"/>
-      </right>
-      <top style="thin">
-        <color rgb="FFB2B2B2"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FFB2B2B2"/>
+        <color theme="4"/>
       </bottom>
       <diagonal/>
     </border>
@@ -901,162 +918,151 @@
       </bottom>
       <diagonal/>
     </border>
-    <border>
-      <left/>
-      <right/>
-      <top style="thin">
-        <color theme="4"/>
-      </top>
-      <bottom style="double">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="17" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="25" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="5" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="44" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="22" borderId="6" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="6" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="5" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="6" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="6" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="44" fontId="9" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="7" borderId="5" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="32" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="6" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="176" fontId="9" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="42" fontId="9" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="177" fontId="9" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="3" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="9" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="21" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="177" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="42" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="176" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="13" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="9" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
@@ -1065,19 +1071,25 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
@@ -1091,9 +1103,6 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1104,9 +1113,6 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
   </cellXfs>
   <cellStyles count="49">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1423,8 +1429,8 @@
   <sheetPr/>
   <dimension ref="A1:O33"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="145" zoomScaleNormal="145" topLeftCell="C1" workbookViewId="0">
-      <selection activeCell="G1" sqref="G$1:G$1048576"/>
+    <sheetView tabSelected="1" zoomScale="145" zoomScaleNormal="145" topLeftCell="D1" workbookViewId="0">
+      <selection activeCell="K15" sqref="K15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10" defaultRowHeight="12.75"/>
@@ -1434,11 +1440,12 @@
     <col min="3" max="3" width="14.1428571428571" customWidth="1"/>
     <col min="4" max="4" width="20.1428571428571" customWidth="1"/>
     <col min="5" max="5" width="10.2857142857143" customWidth="1"/>
-    <col min="6" max="6" width="12.5714285714286" style="13" customWidth="1"/>
-    <col min="7" max="7" width="15.5619047619048" style="13" customWidth="1"/>
+    <col min="6" max="6" width="12.5714285714286" style="14" customWidth="1"/>
+    <col min="7" max="7" width="15.5619047619048" style="14" customWidth="1"/>
     <col min="8" max="8" width="72.0095238095238" customWidth="1"/>
     <col min="9" max="9" width="55" customWidth="1"/>
-    <col min="10" max="11" width="14.6761904761905" customWidth="1"/>
+    <col min="10" max="10" width="14.6761904761905" customWidth="1"/>
+    <col min="11" max="11" width="23.9428571428571" customWidth="1"/>
     <col min="12" max="12" width="8.14285714285714" customWidth="1"/>
     <col min="13" max="13" width="8.57142857142857" customWidth="1"/>
     <col min="14" max="14" width="46.4285714285714" style="1" customWidth="1"/>
@@ -1461,10 +1468,10 @@
       <c r="E1" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="13" t="s">
+      <c r="F1" s="14" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="13" t="s">
+      <c r="G1" s="14" t="s">
         <v>6</v>
       </c>
       <c r="H1" s="1" t="s">
@@ -1485,7 +1492,7 @@
       <c r="M1" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="N1" s="13" t="s">
+      <c r="N1" s="14" t="s">
         <v>13</v>
       </c>
       <c r="O1" t="s">
@@ -1498,13 +1505,13 @@
       </c>
       <c r="B2" s="1"/>
       <c r="C2" s="1"/>
-      <c r="D2" s="14" t="s">
+      <c r="D2" s="15" t="s">
         <v>16</v>
       </c>
-      <c r="E2" s="14" t="s">
+      <c r="E2" s="15" t="s">
         <v>17</v>
       </c>
-      <c r="H2" s="14" t="s">
+      <c r="H2" s="15" t="s">
         <v>18</v>
       </c>
       <c r="I2" t="s">
@@ -1518,19 +1525,21 @@
       <c r="M2" s="1" t="b">
         <v>1</v>
       </c>
-      <c r="N2" s="13"/>
+      <c r="N2" s="14"/>
     </row>
     <row r="3" spans="1:14">
-      <c r="A3" s="1"/>
+      <c r="A3" s="1" t="s">
+        <v>15</v>
+      </c>
       <c r="B3" s="1"/>
       <c r="C3" s="1"/>
-      <c r="D3" s="14" t="s">
+      <c r="D3" s="15" t="s">
         <v>20</v>
       </c>
-      <c r="E3" s="14" t="s">
+      <c r="E3" s="15" t="s">
         <v>17</v>
       </c>
-      <c r="H3" s="14" t="s">
+      <c r="H3" s="15" t="s">
         <v>21</v>
       </c>
       <c r="I3" t="s">
@@ -1544,7 +1553,7 @@
       <c r="M3" s="1" t="b">
         <v>1</v>
       </c>
-      <c r="N3" s="13"/>
+      <c r="N3" s="14"/>
     </row>
     <row r="4" spans="1:13">
       <c r="A4" s="1" t="s">
@@ -1562,8 +1571,8 @@
       <c r="I4" t="s">
         <v>25</v>
       </c>
-      <c r="J4" s="16"/>
-      <c r="K4" s="16"/>
+      <c r="J4" s="17"/>
+      <c r="K4" s="17"/>
       <c r="L4" t="b">
         <v>1</v>
       </c>
@@ -1572,7 +1581,9 @@
       </c>
     </row>
     <row r="5" spans="1:13">
-      <c r="A5" s="1"/>
+      <c r="A5" s="1" t="s">
+        <v>15</v>
+      </c>
       <c r="D5" t="s">
         <v>26</v>
       </c>
@@ -1585,8 +1596,8 @@
       <c r="I5" t="s">
         <v>28</v>
       </c>
-      <c r="J5" s="16"/>
-      <c r="K5" s="16"/>
+      <c r="J5" s="17"/>
+      <c r="K5" s="17"/>
       <c r="L5" t="b">
         <v>1</v>
       </c>
@@ -1595,9 +1606,7 @@
       </c>
     </row>
     <row r="6" spans="1:12">
-      <c r="A6" s="1" t="s">
-        <v>15</v>
-      </c>
+      <c r="A6" s="1"/>
       <c r="D6" t="s">
         <v>29</v>
       </c>
@@ -1610,8 +1619,8 @@
       <c r="I6" t="s">
         <v>32</v>
       </c>
-      <c r="J6" s="16"/>
-      <c r="K6" s="16"/>
+      <c r="J6" s="17"/>
+      <c r="K6" s="17"/>
       <c r="L6" t="b">
         <v>1</v>
       </c>
@@ -1624,18 +1633,18 @@
       <c r="E7" t="s">
         <v>34</v>
       </c>
-      <c r="F7" s="15" t="s">
+      <c r="F7" s="16" t="s">
         <v>35</v>
       </c>
-      <c r="G7" s="15"/>
+      <c r="G7" s="16"/>
       <c r="H7" t="s">
         <v>36</v>
       </c>
       <c r="I7" t="s">
         <v>37</v>
       </c>
-      <c r="J7" s="16"/>
-      <c r="K7" s="16"/>
+      <c r="J7" s="17"/>
+      <c r="K7" s="17"/>
       <c r="L7" t="b">
         <v>1</v>
       </c>
@@ -1648,7 +1657,7 @@
       <c r="E8" t="s">
         <v>34</v>
       </c>
-      <c r="F8" s="13" t="s">
+      <c r="F8" s="14" t="s">
         <v>39</v>
       </c>
       <c r="H8" t="s">
@@ -1657,8 +1666,8 @@
       <c r="I8" t="s">
         <v>41</v>
       </c>
-      <c r="J8" s="16"/>
-      <c r="K8" s="16"/>
+      <c r="J8" s="17"/>
+      <c r="K8" s="17"/>
       <c r="L8" t="b">
         <v>1</v>
       </c>
@@ -1675,7 +1684,7 @@
       <c r="E9" t="s">
         <v>34</v>
       </c>
-      <c r="F9" s="13" t="s">
+      <c r="F9" s="14" t="s">
         <v>39</v>
       </c>
       <c r="H9" t="s">
@@ -1684,8 +1693,8 @@
       <c r="I9" t="s">
         <v>45</v>
       </c>
-      <c r="J9" s="16"/>
-      <c r="K9" s="16"/>
+      <c r="J9" s="17"/>
+      <c r="K9" s="17"/>
       <c r="L9" t="b">
         <v>1</v>
       </c>
@@ -1708,8 +1717,8 @@
       <c r="I10" t="s">
         <v>49</v>
       </c>
-      <c r="J10" s="16"/>
-      <c r="K10" s="16"/>
+      <c r="J10" s="17"/>
+      <c r="K10" s="17"/>
       <c r="L10" t="b">
         <v>1</v>
       </c>
@@ -1725,18 +1734,18 @@
       <c r="E11" t="s">
         <v>34</v>
       </c>
-      <c r="F11" s="15" t="s">
+      <c r="F11" s="16" t="s">
         <v>51</v>
       </c>
-      <c r="G11" s="15"/>
+      <c r="G11" s="16"/>
       <c r="H11" t="s">
         <v>52</v>
       </c>
       <c r="I11" t="s">
         <v>53</v>
       </c>
-      <c r="J11" s="16"/>
-      <c r="K11" s="16"/>
+      <c r="J11" s="17"/>
+      <c r="K11" s="17"/>
       <c r="L11" t="b">
         <v>1</v>
       </c>
@@ -1758,8 +1767,8 @@
       <c r="I12" t="s">
         <v>57</v>
       </c>
-      <c r="J12" s="16"/>
-      <c r="K12" s="16"/>
+      <c r="J12" s="17"/>
+      <c r="K12" s="17"/>
       <c r="L12" t="b">
         <v>1</v>
       </c>
@@ -1775,18 +1784,18 @@
       <c r="E13" t="s">
         <v>34</v>
       </c>
-      <c r="F13" s="15" t="s">
+      <c r="F13" s="16" t="s">
         <v>39</v>
       </c>
-      <c r="G13" s="15"/>
+      <c r="G13" s="16"/>
       <c r="H13" t="s">
         <v>59</v>
       </c>
       <c r="I13" t="s">
         <v>60</v>
       </c>
-      <c r="J13" s="16"/>
-      <c r="K13" s="16"/>
+      <c r="J13" s="17"/>
+      <c r="K13" s="17"/>
       <c r="L13" t="b">
         <v>1</v>
       </c>
@@ -1802,16 +1811,16 @@
       <c r="E14" t="s">
         <v>30</v>
       </c>
-      <c r="F14" s="15"/>
-      <c r="G14" s="15"/>
+      <c r="F14" s="16"/>
+      <c r="G14" s="16"/>
       <c r="H14" t="s">
         <v>62</v>
       </c>
       <c r="I14" t="s">
         <v>63</v>
       </c>
-      <c r="J14" s="16"/>
-      <c r="K14" s="16"/>
+      <c r="J14" s="17"/>
+      <c r="K14" s="17"/>
       <c r="L14" t="b">
         <v>1</v>
       </c>
@@ -1827,16 +1836,16 @@
       <c r="E15" t="s">
         <v>30</v>
       </c>
-      <c r="F15" s="15"/>
-      <c r="G15" s="15"/>
+      <c r="F15" s="16"/>
+      <c r="G15" s="16"/>
       <c r="H15" t="s">
         <v>66</v>
       </c>
       <c r="I15" t="s">
         <v>67</v>
       </c>
-      <c r="J15" s="16"/>
-      <c r="K15" s="16" t="s">
+      <c r="J15" s="17"/>
+      <c r="K15" s="17" t="s">
         <v>68</v>
       </c>
       <c r="L15" t="b">
@@ -1848,7 +1857,7 @@
       <c r="N15" s="1" t="s">
         <v>42</v>
       </c>
-      <c r="O15" s="17"/>
+      <c r="O15" s="1"/>
     </row>
     <row r="16" spans="1:13">
       <c r="A16" s="1" t="s">
@@ -1866,8 +1875,8 @@
       <c r="I16" t="s">
         <v>73</v>
       </c>
-      <c r="J16" s="16"/>
-      <c r="K16" s="16"/>
+      <c r="J16" s="17"/>
+      <c r="K16" s="17"/>
       <c r="L16" t="b">
         <v>1</v>
       </c>
@@ -1891,8 +1900,8 @@
       <c r="I17" t="s">
         <v>77</v>
       </c>
-      <c r="J17" s="16"/>
-      <c r="K17" s="16"/>
+      <c r="J17" s="17"/>
+      <c r="K17" s="17"/>
       <c r="L17" t="b">
         <v>1</v>
       </c>
@@ -1916,8 +1925,8 @@
       <c r="I18" t="s">
         <v>80</v>
       </c>
-      <c r="J18" s="16"/>
-      <c r="K18" s="16"/>
+      <c r="J18" s="17"/>
+      <c r="K18" s="17"/>
       <c r="L18" t="b">
         <v>1</v>
       </c>
@@ -1927,23 +1936,23 @@
     </row>
     <row r="19" spans="1:11">
       <c r="A19" s="1"/>
-      <c r="J19" s="16"/>
-      <c r="K19" s="16"/>
+      <c r="J19" s="17"/>
+      <c r="K19" s="17"/>
     </row>
     <row r="20" spans="1:11">
       <c r="A20" s="1"/>
-      <c r="J20" s="16"/>
-      <c r="K20" s="16"/>
+      <c r="J20" s="17"/>
+      <c r="K20" s="17"/>
     </row>
     <row r="21" spans="1:11">
       <c r="A21" s="1"/>
-      <c r="J21" s="16"/>
-      <c r="K21" s="16"/>
+      <c r="J21" s="17"/>
+      <c r="K21" s="17"/>
     </row>
     <row r="22" spans="1:11">
       <c r="A22" s="1"/>
-      <c r="J22" s="16"/>
-      <c r="K22" s="16"/>
+      <c r="J22" s="17"/>
+      <c r="K22" s="17"/>
     </row>
     <row r="23" spans="1:1">
       <c r="A23" s="1"/>
@@ -1991,7 +2000,7 @@
   <dimension ref="A1:E47"/>
   <sheetViews>
     <sheetView zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="B10" sqref="B10"/>
+      <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.14285714285714" defaultRowHeight="12.75" outlineLevelCol="4"/>
@@ -2023,14 +2032,14 @@
       <c r="A2" t="s">
         <v>39</v>
       </c>
-      <c r="B2" s="1" t="b">
-        <v>1</v>
+      <c r="B2" s="2" t="s">
+        <v>82</v>
       </c>
       <c r="C2" t="s">
-        <v>82</v>
+        <v>83</v>
       </c>
       <c r="D2" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="E2" s="1"/>
     </row>
@@ -2038,312 +2047,312 @@
       <c r="A3" t="s">
         <v>39</v>
       </c>
-      <c r="B3" s="1" t="b">
-        <v>0</v>
+      <c r="B3" s="2" t="s">
+        <v>85</v>
       </c>
       <c r="C3" t="s">
-        <v>84</v>
+        <v>86</v>
       </c>
       <c r="D3" t="s">
-        <v>85</v>
+        <v>87</v>
       </c>
       <c r="E3" s="1"/>
     </row>
     <row r="4" spans="1:5">
-      <c r="A4" s="2" t="s">
-        <v>86</v>
-      </c>
-      <c r="B4" s="3" t="s">
-        <v>87</v>
-      </c>
-      <c r="C4" s="2" t="s">
+      <c r="A4" s="3" t="s">
         <v>88</v>
       </c>
-      <c r="D4" s="2" t="s">
+      <c r="B4" s="4" t="s">
         <v>89</v>
       </c>
-      <c r="E4" s="2"/>
+      <c r="C4" s="3" t="s">
+        <v>90</v>
+      </c>
+      <c r="D4" s="3" t="s">
+        <v>91</v>
+      </c>
+      <c r="E4" s="3"/>
     </row>
     <row r="5" spans="1:5">
-      <c r="A5" s="2" t="s">
-        <v>86</v>
-      </c>
-      <c r="B5" s="3" t="s">
-        <v>90</v>
-      </c>
-      <c r="C5" s="2" t="s">
-        <v>91</v>
-      </c>
-      <c r="D5" s="2" t="s">
+      <c r="A5" s="3" t="s">
+        <v>88</v>
+      </c>
+      <c r="B5" s="4" t="s">
         <v>92</v>
       </c>
-      <c r="E5" s="2"/>
+      <c r="C5" s="3" t="s">
+        <v>93</v>
+      </c>
+      <c r="D5" s="3" t="s">
+        <v>94</v>
+      </c>
+      <c r="E5" s="3"/>
     </row>
     <row r="6" spans="1:5">
-      <c r="A6" s="2" t="s">
+      <c r="A6" s="3" t="s">
         <v>51</v>
       </c>
-      <c r="B6" s="3" t="s">
-        <v>93</v>
-      </c>
-      <c r="C6" s="2" t="s">
-        <v>94</v>
-      </c>
-      <c r="D6" s="2" t="s">
+      <c r="B6" s="4" t="s">
         <v>95</v>
       </c>
-      <c r="E6" s="12"/>
+      <c r="C6" s="3" t="s">
+        <v>96</v>
+      </c>
+      <c r="D6" s="3" t="s">
+        <v>97</v>
+      </c>
+      <c r="E6" s="4"/>
     </row>
     <row r="7" spans="1:4">
-      <c r="A7" s="2" t="s">
+      <c r="A7" s="3" t="s">
         <v>51</v>
       </c>
-      <c r="B7" s="4" t="s">
-        <v>96</v>
-      </c>
-      <c r="C7" s="5" t="s">
-        <v>97</v>
-      </c>
-      <c r="D7" s="5" t="s">
+      <c r="B7" s="5" t="s">
         <v>98</v>
       </c>
+      <c r="C7" s="6" t="s">
+        <v>99</v>
+      </c>
+      <c r="D7" s="6" t="s">
+        <v>100</v>
+      </c>
     </row>
     <row r="8" spans="1:4">
-      <c r="A8" s="2" t="s">
+      <c r="A8" s="3" t="s">
         <v>51</v>
       </c>
-      <c r="B8" s="4" t="s">
-        <v>99</v>
-      </c>
-      <c r="C8" s="5" t="s">
-        <v>100</v>
-      </c>
-      <c r="D8" s="5" t="s">
+      <c r="B8" s="5" t="s">
         <v>101</v>
       </c>
+      <c r="C8" s="6" t="s">
+        <v>102</v>
+      </c>
+      <c r="D8" s="6" t="s">
+        <v>103</v>
+      </c>
     </row>
     <row r="9" spans="1:4">
-      <c r="A9" s="2" t="s">
+      <c r="A9" s="3" t="s">
         <v>51</v>
       </c>
-      <c r="B9" s="4" t="s">
-        <v>102</v>
-      </c>
-      <c r="C9" s="5" t="s">
-        <v>103</v>
-      </c>
-      <c r="D9" s="5" t="s">
+      <c r="B9" s="5" t="s">
         <v>104</v>
       </c>
+      <c r="C9" s="6" t="s">
+        <v>105</v>
+      </c>
+      <c r="D9" s="6" t="s">
+        <v>106</v>
+      </c>
     </row>
     <row r="10" spans="1:4">
-      <c r="A10" s="6" t="s">
+      <c r="A10" s="7" t="s">
         <v>35</v>
       </c>
-      <c r="B10" s="4" t="s">
-        <v>105</v>
-      </c>
-      <c r="C10" s="5" t="s">
-        <v>106</v>
-      </c>
-      <c r="D10" s="5"/>
+      <c r="B10" s="5" t="s">
+        <v>107</v>
+      </c>
+      <c r="C10" s="6" t="s">
+        <v>108</v>
+      </c>
+      <c r="D10" s="6"/>
     </row>
     <row r="11" spans="1:4">
-      <c r="A11" s="6" t="s">
+      <c r="A11" s="7" t="s">
         <v>35</v>
       </c>
-      <c r="B11" s="4" t="s">
-        <v>107</v>
-      </c>
-      <c r="C11" s="5" t="s">
-        <v>108</v>
-      </c>
-      <c r="D11" s="5"/>
+      <c r="B11" s="5" t="s">
+        <v>109</v>
+      </c>
+      <c r="C11" s="6" t="s">
+        <v>110</v>
+      </c>
+      <c r="D11" s="6"/>
     </row>
     <row r="12" spans="1:4">
-      <c r="A12" s="6" t="s">
+      <c r="A12" s="7" t="s">
         <v>35</v>
       </c>
-      <c r="B12" s="4" t="s">
-        <v>109</v>
-      </c>
-      <c r="C12" s="5" t="s">
-        <v>110</v>
-      </c>
-      <c r="D12" s="5"/>
+      <c r="B12" s="5" t="s">
+        <v>111</v>
+      </c>
+      <c r="C12" s="6" t="s">
+        <v>112</v>
+      </c>
+      <c r="D12" s="6"/>
     </row>
     <row r="13" spans="1:4">
-      <c r="A13" s="6"/>
-      <c r="B13" s="4"/>
-      <c r="C13" s="5"/>
-      <c r="D13" s="5"/>
+      <c r="A13" s="7"/>
+      <c r="B13" s="8"/>
+      <c r="C13" s="6"/>
+      <c r="D13" s="6"/>
     </row>
     <row r="14" spans="1:4">
-      <c r="A14" s="6"/>
-      <c r="B14" s="4"/>
-      <c r="C14" s="5"/>
-      <c r="D14" s="5"/>
+      <c r="A14" s="7"/>
+      <c r="B14" s="8"/>
+      <c r="C14" s="6"/>
+      <c r="D14" s="6"/>
     </row>
     <row r="16" spans="1:3">
-      <c r="A16" s="7"/>
-      <c r="B16" s="8"/>
-      <c r="C16" s="9"/>
+      <c r="A16" s="9"/>
+      <c r="B16" s="10"/>
+      <c r="C16" s="11"/>
     </row>
     <row r="17" spans="1:3">
-      <c r="A17" s="7"/>
-      <c r="B17" s="8"/>
-      <c r="C17" s="9"/>
+      <c r="A17" s="9"/>
+      <c r="B17" s="10"/>
+      <c r="C17" s="11"/>
     </row>
     <row r="18" spans="1:3">
-      <c r="A18" s="7"/>
-      <c r="B18" s="8"/>
-      <c r="C18" s="9"/>
+      <c r="A18" s="9"/>
+      <c r="B18" s="10"/>
+      <c r="C18" s="11"/>
     </row>
     <row r="19" spans="1:3">
-      <c r="A19" s="7"/>
-      <c r="B19" s="8"/>
-      <c r="C19" s="10"/>
+      <c r="A19" s="9"/>
+      <c r="B19" s="10"/>
+      <c r="C19" s="12"/>
     </row>
     <row r="20" spans="1:3">
-      <c r="A20" s="7"/>
-      <c r="B20" s="8"/>
-      <c r="C20" s="9"/>
+      <c r="A20" s="9"/>
+      <c r="B20" s="10"/>
+      <c r="C20" s="11"/>
     </row>
     <row r="21" spans="1:3">
-      <c r="A21" s="7"/>
-      <c r="B21" s="8"/>
-      <c r="C21" s="9"/>
+      <c r="A21" s="9"/>
+      <c r="B21" s="10"/>
+      <c r="C21" s="11"/>
     </row>
     <row r="22" spans="1:3">
-      <c r="A22" s="7"/>
-      <c r="B22" s="8"/>
-      <c r="C22" s="9"/>
+      <c r="A22" s="9"/>
+      <c r="B22" s="10"/>
+      <c r="C22" s="11"/>
     </row>
     <row r="23" spans="1:3">
-      <c r="A23" s="7"/>
-      <c r="B23" s="8"/>
-      <c r="C23" s="9"/>
+      <c r="A23" s="9"/>
+      <c r="B23" s="10"/>
+      <c r="C23" s="11"/>
     </row>
     <row r="24" spans="1:5">
-      <c r="A24" s="7"/>
-      <c r="B24" s="8"/>
-      <c r="C24" s="10"/>
-      <c r="E24" s="9"/>
+      <c r="A24" s="9"/>
+      <c r="B24" s="10"/>
+      <c r="C24" s="12"/>
+      <c r="E24" s="11"/>
     </row>
     <row r="25" spans="1:5">
-      <c r="A25" s="7"/>
-      <c r="E25" s="9"/>
+      <c r="A25" s="9"/>
+      <c r="E25" s="11"/>
     </row>
     <row r="26" spans="1:5">
-      <c r="A26" s="6"/>
-      <c r="B26" s="11"/>
-      <c r="C26" s="5"/>
-      <c r="D26" s="5"/>
-      <c r="E26" s="9"/>
+      <c r="A26" s="7"/>
+      <c r="B26" s="13"/>
+      <c r="C26" s="6"/>
+      <c r="D26" s="6"/>
+      <c r="E26" s="11"/>
     </row>
     <row r="27" spans="1:5">
-      <c r="A27" s="6"/>
-      <c r="B27" s="11"/>
-      <c r="C27" s="5"/>
-      <c r="D27" s="5"/>
-      <c r="E27" s="10"/>
+      <c r="A27" s="7"/>
+      <c r="B27" s="13"/>
+      <c r="C27" s="6"/>
+      <c r="D27" s="6"/>
+      <c r="E27" s="12"/>
     </row>
     <row r="28" spans="1:5">
-      <c r="A28" s="6"/>
-      <c r="B28" s="11"/>
-      <c r="C28" s="5"/>
-      <c r="D28" s="5"/>
-      <c r="E28" s="9"/>
+      <c r="A28" s="7"/>
+      <c r="B28" s="13"/>
+      <c r="C28" s="6"/>
+      <c r="D28" s="6"/>
+      <c r="E28" s="11"/>
     </row>
     <row r="29" spans="1:5">
-      <c r="A29" s="6"/>
-      <c r="B29" s="11"/>
-      <c r="C29" s="5"/>
-      <c r="D29" s="5"/>
-      <c r="E29" s="9"/>
+      <c r="A29" s="7"/>
+      <c r="B29" s="13"/>
+      <c r="C29" s="6"/>
+      <c r="D29" s="6"/>
+      <c r="E29" s="11"/>
     </row>
     <row r="30" spans="1:5">
-      <c r="A30" s="6"/>
-      <c r="B30" s="11"/>
-      <c r="C30" s="5"/>
-      <c r="D30" s="5"/>
-      <c r="E30" s="9"/>
+      <c r="A30" s="7"/>
+      <c r="B30" s="13"/>
+      <c r="C30" s="6"/>
+      <c r="D30" s="6"/>
+      <c r="E30" s="11"/>
     </row>
     <row r="31" spans="1:5">
-      <c r="A31" s="7"/>
-      <c r="B31" s="8"/>
-      <c r="C31" s="9"/>
-      <c r="D31" s="9"/>
-      <c r="E31" s="10"/>
+      <c r="A31" s="9"/>
+      <c r="B31" s="10"/>
+      <c r="C31" s="11"/>
+      <c r="D31" s="11"/>
+      <c r="E31" s="12"/>
     </row>
     <row r="32" spans="1:5">
-      <c r="A32" s="7"/>
-      <c r="B32" s="8"/>
-      <c r="C32" s="9"/>
-      <c r="D32" s="9"/>
-      <c r="E32" s="9"/>
+      <c r="A32" s="9"/>
+      <c r="B32" s="10"/>
+      <c r="C32" s="11"/>
+      <c r="D32" s="11"/>
+      <c r="E32" s="11"/>
     </row>
     <row r="33" spans="1:5">
-      <c r="A33" s="7"/>
-      <c r="B33" s="8"/>
-      <c r="C33" s="9"/>
-      <c r="D33" s="9"/>
-      <c r="E33" s="9"/>
+      <c r="A33" s="9"/>
+      <c r="B33" s="10"/>
+      <c r="C33" s="11"/>
+      <c r="D33" s="11"/>
+      <c r="E33" s="11"/>
     </row>
     <row r="34" spans="1:5">
-      <c r="A34" s="7"/>
-      <c r="B34" s="8"/>
-      <c r="C34" s="9"/>
-      <c r="D34" s="9"/>
-      <c r="E34" s="9"/>
+      <c r="A34" s="9"/>
+      <c r="B34" s="10"/>
+      <c r="C34" s="11"/>
+      <c r="D34" s="11"/>
+      <c r="E34" s="11"/>
     </row>
     <row r="35" spans="1:5">
-      <c r="A35" s="7"/>
-      <c r="B35" s="8"/>
-      <c r="C35" s="9"/>
-      <c r="D35" s="9"/>
-      <c r="E35" s="9"/>
+      <c r="A35" s="9"/>
+      <c r="B35" s="10"/>
+      <c r="C35" s="11"/>
+      <c r="D35" s="11"/>
+      <c r="E35" s="11"/>
     </row>
     <row r="36" spans="1:5">
-      <c r="A36" s="7"/>
-      <c r="B36" s="8"/>
-      <c r="C36" s="9"/>
-      <c r="D36" s="9"/>
-      <c r="E36" s="9"/>
+      <c r="A36" s="9"/>
+      <c r="B36" s="10"/>
+      <c r="C36" s="11"/>
+      <c r="D36" s="11"/>
+      <c r="E36" s="11"/>
     </row>
     <row r="37" spans="1:5">
-      <c r="A37" s="7"/>
-      <c r="B37" s="8"/>
-      <c r="C37" s="9"/>
-      <c r="D37" s="9"/>
-      <c r="E37" s="9"/>
+      <c r="A37" s="9"/>
+      <c r="B37" s="10"/>
+      <c r="C37" s="11"/>
+      <c r="D37" s="11"/>
+      <c r="E37" s="11"/>
     </row>
     <row r="39" spans="5:5">
-      <c r="E39" s="9"/>
+      <c r="E39" s="11"/>
     </row>
     <row r="40" spans="5:5">
-      <c r="E40" s="9"/>
+      <c r="E40" s="11"/>
     </row>
     <row r="41" spans="5:5">
-      <c r="E41" s="9"/>
+      <c r="E41" s="11"/>
     </row>
     <row r="42" spans="5:5">
-      <c r="E42" s="10"/>
+      <c r="E42" s="12"/>
     </row>
     <row r="43" spans="5:5">
-      <c r="E43" s="9"/>
+      <c r="E43" s="11"/>
     </row>
     <row r="44" spans="5:5">
-      <c r="E44" s="9"/>
+      <c r="E44" s="11"/>
     </row>
     <row r="45" spans="5:5">
-      <c r="E45" s="9"/>
+      <c r="E45" s="11"/>
     </row>
     <row r="46" spans="5:5">
-      <c r="E46" s="9"/>
+      <c r="E46" s="11"/>
     </row>
     <row r="47" spans="5:5">
-      <c r="E47" s="9"/>
+      <c r="E47" s="11"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
@@ -2358,7 +2367,7 @@
   <dimension ref="A1:C2"/>
   <sheetViews>
     <sheetView zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.14285714285714" defaultRowHeight="12.75" outlineLevelRow="1" outlineLevelCol="2"/>
@@ -2370,24 +2379,24 @@
   <sheetData>
     <row r="1" spans="1:3">
       <c r="A1" s="1" t="s">
-        <v>111</v>
+        <v>113</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>112</v>
+        <v>114</v>
       </c>
       <c r="C1" t="s">
-        <v>113</v>
+        <v>115</v>
       </c>
     </row>
     <row r="2" spans="1:3">
       <c r="A2" t="s">
-        <v>114</v>
+        <v>116</v>
       </c>
       <c r="B2" t="s">
-        <v>115</v>
+        <v>117</v>
       </c>
       <c r="C2" t="s">
-        <v>116</v>
+        <v>118</v>
       </c>
     </row>
   </sheetData>

</xml_diff>